<commit_message>
latest update from main
</commit_message>
<xml_diff>
--- a/tests/testMaterials/CDS_SPARSE_2014_2015.xlsx
+++ b/tests/testMaterials/CDS_SPARSE_2014_2015.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\tests\testMaterials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D44425-F30B-4796-AAA0-2337F044CBA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B823EB1E-0B73-4CE9-8ED7-FC3EB89B4FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -115,10 +115,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,8 +402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -424,7 +425,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -468,7 +469,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>83</v>
       </c>
       <c r="B2">
@@ -512,7 +513,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>199</v>
       </c>
       <c r="B3">
@@ -556,7 +557,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>300</v>
       </c>
       <c r="B4">
@@ -600,7 +601,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>582</v>
       </c>
       <c r="B5">
@@ -644,7 +645,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>0</v>
       </c>
       <c r="B6">
@@ -688,7 +689,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="3">
         <v>0</v>
       </c>
       <c r="B7">
@@ -732,7 +733,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>1</v>
       </c>
       <c r="B8">
@@ -776,7 +777,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>1</v>
       </c>
       <c r="B9">
@@ -820,7 +821,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>83</v>
       </c>
       <c r="B10">
@@ -864,7 +865,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="3">
         <v>199</v>
       </c>
       <c r="B11">
@@ -908,7 +909,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>299</v>
       </c>
       <c r="B12">
@@ -952,7 +953,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="3">
         <v>581</v>
       </c>
       <c r="B13">
@@ -996,7 +997,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="3">
         <v>61</v>
       </c>
       <c r="B14">
@@ -1040,7 +1041,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="3">
         <v>144</v>
       </c>
       <c r="B15">
@@ -1084,7 +1085,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="3">
         <v>220</v>
       </c>
       <c r="B16">
@@ -1128,7 +1129,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="A17" s="3">
         <v>425</v>
       </c>
       <c r="B17">
@@ -1172,7 +1173,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="3">
         <v>7</v>
       </c>
       <c r="B18">
@@ -1216,7 +1217,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="3">
         <v>9</v>
       </c>
       <c r="B19">
@@ -1260,7 +1261,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="A20" s="3">
         <v>33</v>
       </c>
       <c r="B20">
@@ -1304,7 +1305,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="A21" s="3">
         <v>49</v>
       </c>
       <c r="B21">
@@ -1348,7 +1349,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="A22" s="3">
         <v>1</v>
       </c>
       <c r="B22">
@@ -1392,7 +1393,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="A23" s="3">
         <v>5</v>
       </c>
       <c r="B23">
@@ -1436,7 +1437,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24">
+      <c r="A24" s="3">
         <v>3</v>
       </c>
       <c r="B24">
@@ -1480,7 +1481,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25">
+      <c r="A25" s="3">
         <v>9</v>
       </c>
       <c r="B25">
@@ -1524,7 +1525,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26">
+      <c r="A26" s="3">
         <v>69</v>
       </c>
       <c r="B26">
@@ -1568,7 +1569,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="A27" s="3">
         <v>158</v>
       </c>
       <c r="B27">
@@ -1612,7 +1613,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="A28" s="3">
         <v>256</v>
       </c>
       <c r="B28">
@@ -1656,7 +1657,7 @@
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A29">
+      <c r="A29" s="3">
         <v>483</v>
       </c>
       <c r="B29">
@@ -1700,7 +1701,7 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30">
+      <c r="A30" s="3">
         <v>83</v>
       </c>
       <c r="B30">
@@ -1744,7 +1745,7 @@
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31">
+      <c r="A31" s="3">
         <v>79</v>
       </c>
       <c r="B31">
@@ -1788,7 +1789,7 @@
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A32">
+      <c r="A32" s="3">
         <v>85.6</v>
       </c>
       <c r="B32">
@@ -1832,7 +1833,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33">
+      <c r="A33" s="3">
         <v>83</v>
       </c>
       <c r="B33">
@@ -1876,6 +1877,7 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" s="3"/>
       <c r="H34" s="1"/>
     </row>
   </sheetData>

</xml_diff>